<commit_message>
MY OWN PROJECT PUSH
</commit_message>
<xml_diff>
--- a/Own_FrameWork_On_CRM_GUI/TestData/testscriptdata.xlsx
+++ b/Own_FrameWork_On_CRM_GUI/TestData/testscriptdata.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
     <sheet name="TP-20" sheetId="6" r:id="rId6"/>
     <sheet name="TP-21" sheetId="7" r:id="rId7"/>
-    <sheet name="Opportunity" sheetId="8" r:id="rId8"/>
+    <sheet name="OwnTest" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="111">
   <si>
     <t>TC_ID</t>
   </si>
@@ -310,6 +310,63 @@
   </si>
   <si>
     <t>BambooTree_</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>RelatedTo</t>
+  </si>
+  <si>
+    <t>Maiyan Arpitha_</t>
+  </si>
+  <si>
+    <t>Contacts</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>CreateProducts</t>
+  </si>
+  <si>
+    <t>NeckBand_</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>CreateProductsWithVendor</t>
+  </si>
+  <si>
+    <t>SonShine_</t>
+  </si>
+  <si>
+    <t>CampaignName</t>
+  </si>
+  <si>
+    <t>TC_05</t>
+  </si>
+  <si>
+    <t>CreateCampaign</t>
+  </si>
+  <si>
+    <t>Purple Tulips_</t>
+  </si>
+  <si>
+    <t>TroubleTicketTitle</t>
+  </si>
+  <si>
+    <t>TC_06</t>
+  </si>
+  <si>
+    <t>CreateTroubleTicket</t>
+  </si>
+  <si>
+    <t>Quality is Not as Expected_</t>
   </si>
 </sst>
 </file>
@@ -962,10 +1019,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1037,13 +1096,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
-<customStorage xmlns="https://web.wps.cn/et/2018/main">
-  <book/>
-  <sheets/>
-</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1400,7 +1452,7 @@
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1480,17 +1532,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1506,15 +1558,15 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1530,19 +1582,19 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1599,7 +1651,7 @@
       <c r="A2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C2" t="s">
@@ -1610,7 +1662,7 @@
       <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C3" t="s">
@@ -1621,7 +1673,7 @@
       <c r="A4" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C4" t="s">
@@ -1629,8 +1681,8 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="9"/>
     </row>
     <row r="41" spans="9:9">
       <c r="I41" t="s">
@@ -1670,7 +1722,7 @@
       <c r="A2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1678,7 +1730,7 @@
       <c r="A3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1714,7 +1766,7 @@
       <c r="A2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1722,7 +1774,7 @@
       <c r="A3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1730,7 +1782,7 @@
       <c r="A4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1738,7 +1790,7 @@
       <c r="A5" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1746,7 +1798,7 @@
       <c r="A6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1754,7 +1806,7 @@
       <c r="A7" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1795,7 +1847,7 @@
       <c r="A2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="7">
         <v>44167</v>
       </c>
       <c r="C2">
@@ -1806,7 +1858,7 @@
       <c r="A3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="7">
         <v>44168</v>
       </c>
       <c r="C3">
@@ -1817,7 +1869,7 @@
       <c r="A4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="7">
         <v>44169</v>
       </c>
       <c r="C4">
@@ -1828,7 +1880,7 @@
       <c r="A5" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="7">
         <v>44170</v>
       </c>
       <c r="C5">
@@ -1839,7 +1891,7 @@
       <c r="A6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="7">
         <v>44171</v>
       </c>
       <c r="C6">
@@ -1850,7 +1902,7 @@
       <c r="A7" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="7">
         <v>44172</v>
       </c>
       <c r="C7">
@@ -1861,7 +1913,7 @@
       <c r="A8" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="7">
         <v>44173</v>
       </c>
       <c r="C8">
@@ -1872,7 +1924,7 @@
       <c r="A9" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="7">
         <v>44174</v>
       </c>
       <c r="C9">
@@ -1883,7 +1935,7 @@
       <c r="A10" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="7">
         <v>44175</v>
       </c>
       <c r="C10">
@@ -1894,7 +1946,7 @@
       <c r="A11" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="7">
         <v>44176</v>
       </c>
       <c r="C11">
@@ -1918,228 +1970,228 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="2" width="11.8571428571429" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.4285714285714" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.14285714285714" style="3"/>
+    <col min="1" max="2" width="11.8571428571429" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.4285714285714" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="9.14285714285714" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="6">
         <v>45993</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>30000</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="6">
         <v>45994</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>80000</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="6">
         <v>45995</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>25000</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="6">
         <v>45996</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
         <v>75000</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>45997</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>10000</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="6">
         <v>45998</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>60000</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="6">
         <v>45999</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="5">
         <v>79000</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="6">
         <v>46000</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>35000</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="6">
         <v>46001</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="5">
         <v>97000</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="6">
         <v>46002</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="5">
         <v>13500</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="6">
         <v>46003</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="5">
         <v>27000</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="6">
         <v>46004</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="5">
         <v>16250</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="6">
         <v>46005</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="5">
         <v>5500</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="6">
         <v>46006</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="5">
         <v>60000</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="6">
         <v>46007</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="5">
         <v>79000</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="6">
         <v>46008</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="5">
         <v>35000</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="6">
         <v>46009</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="5">
         <v>97000</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="6">
         <v>46010</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="5">
         <v>13500</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="6">
         <v>46011</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="5">
         <v>13501</v>
       </c>
     </row>
@@ -2152,17 +2204,18 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="2" max="2" width="20.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="30.5714285714286" customWidth="1"/>
     <col min="3" max="3" width="23.5714285714286" customWidth="1"/>
     <col min="4" max="4" width="23.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="27.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2170,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>89</v>
@@ -2198,16 +2251,16 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2218,13 +2271,125 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" customFormat="1" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" customFormat="1" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>